<commit_message>
1, Improve adaptive interpolation delay algorithm
</commit_message>
<xml_diff>
--- a/Doc/NetworkTest.xlsx
+++ b/Doc/NetworkTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>时延抖动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -568,6 +568,24 @@
   <si>
     <t>WIFI</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均时延(ms)</t>
+  </si>
+  <si>
+    <t>时延抖动</t>
+  </si>
+  <si>
+    <t>丢包率</t>
+  </si>
+  <si>
+    <t>RTT</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>CAT</t>
   </si>
 </sst>
 </file>
@@ -900,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G169"/>
+  <dimension ref="A1:N169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I1" sqref="I1:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -913,7 +931,7 @@
     <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -932,8 +950,26 @@
       <c r="G1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>33</v>
       </c>
@@ -952,8 +988,26 @@
       <c r="G2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>32</v>
+      </c>
+      <c r="M2">
+        <v>35</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>66</v>
       </c>
@@ -969,8 +1023,26 @@
       <c r="F3">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I3">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>63</v>
+      </c>
+      <c r="M3">
+        <v>44</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>100</v>
       </c>
@@ -986,8 +1058,26 @@
       <c r="F4">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>230</v>
+      </c>
+      <c r="M4">
+        <v>294</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>200</v>
       </c>
@@ -1000,8 +1090,26 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>573</v>
+      </c>
+      <c r="M5">
+        <v>739</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>500</v>
       </c>
@@ -1011,8 +1119,26 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I6">
+        <v>500</v>
+      </c>
+      <c r="J6">
+        <v>200</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <v>2176</v>
+      </c>
+      <c r="M6">
+        <v>3102</v>
+      </c>
+      <c r="N6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -1022,8 +1148,17 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>500</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2000</v>
       </c>
@@ -1031,42 +1166,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E16" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
1, Update test results
</commit_message>
<xml_diff>
--- a/Doc/NetworkTest.xlsx
+++ b/Doc/NetworkTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="186">
   <si>
     <t>时延抖动</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -586,6 +586,13 @@
   </si>
   <si>
     <t>CAT</t>
+  </si>
+  <si>
+    <t>无法测试（原因：UDP）</t>
+  </si>
+  <si>
+    <t>无法测试（原因：UDP）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -921,7 +928,7 @@
   <dimension ref="A1:N169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1155,7 +1162,10 @@
         <v>500</v>
       </c>
       <c r="K7">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -1165,15 +1175,57 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>500</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1361</v>
+      </c>
+      <c r="M8">
+        <v>482</v>
+      </c>
+      <c r="N8">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E9" t="s">
         <v>10</v>
       </c>
+      <c r="I9">
+        <v>2000</v>
+      </c>
+      <c r="J9">
+        <v>1200</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="E10" t="s">
         <v>11</v>
+      </c>
+      <c r="I10">
+        <v>2000</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">

</xml_diff>